<commit_message>
profile creation code completed
</commit_message>
<xml_diff>
--- a/TestData/Datasheet.xlsx
+++ b/TestData/Datasheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{8F0B0128-D35D-4138-AC38-0DE967E36C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{FAA32C94-F658-419A-85A4-A803DE6E95E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1E2BD0BB-FCCA-43DE-A424-1FEE5688881A}"/>
   </bookViews>
@@ -21,248 +21,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>MobileNumber</t>
   </si>
   <si>
-    <t>EventTitle</t>
-  </si>
-  <si>
-    <t>EventDetails</t>
-  </si>
-  <si>
-    <t>ClubTitle</t>
-  </si>
-  <si>
-    <t>ClubDetails</t>
-  </si>
-  <si>
-    <t>ArticleTitle</t>
-  </si>
-  <si>
-    <t>ArticleDesc</t>
-  </si>
-  <si>
-    <t>PollQuestion</t>
-  </si>
-  <si>
-    <t>PollOption1</t>
-  </si>
-  <si>
-    <t>PollOption2</t>
-  </si>
-  <si>
-    <t>PollOption3</t>
-  </si>
-  <si>
-    <t>PollOption4</t>
-  </si>
-  <si>
-    <t>SurveyTitle</t>
-  </si>
-  <si>
-    <t>SurveyDesc</t>
-  </si>
-  <si>
-    <t>SurveyQuest1</t>
-  </si>
-  <si>
-    <t>SurveyOption1Q1</t>
-  </si>
-  <si>
-    <t>SurveyOption1Q2</t>
-  </si>
-  <si>
-    <t>SurveyQuest2</t>
-  </si>
-  <si>
-    <t>SurveyOption2Q2</t>
-  </si>
-  <si>
-    <t>SurveyOption2Q1</t>
-  </si>
-  <si>
-    <t>SurveyOption3Q1</t>
-  </si>
-  <si>
-    <t>SurveyOption4Q1</t>
-  </si>
-  <si>
-    <t>SurveyQuest3</t>
-  </si>
-  <si>
-    <t>QueryDesc</t>
-  </si>
-  <si>
-    <t>QueryQuest</t>
-  </si>
-  <si>
     <t>mayurmore2706@gmail.com</t>
   </si>
   <si>
-    <t>CreatePostDesc</t>
-  </si>
-  <si>
-    <t>What must be the top three priorities of a CIO?</t>
-  </si>
-  <si>
-    <t>Cybersecurity and Data Privacy</t>
-  </si>
-  <si>
-    <t>Leveraging AI and Automation</t>
-  </si>
-  <si>
-    <t>Driving Digital Transformation</t>
-  </si>
-  <si>
-    <t>Others</t>
-  </si>
-  <si>
-    <t>Which emerging technology do you think will have the greatest impact on reducing your organization’s environmental footprint?</t>
-  </si>
-  <si>
-    <t>Carbon capture and storage (CCS)
-Internet of Things for monitoring
-Green hydrogen production
-Advanced recycling technologies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Employee Engagement and Satisfaction Survey </t>
-  </si>
-  <si>
-    <t>We value your feedback and want to ensure we are creating the best possible work environment. Please take a few minutes to complete this survey. Your responses are anonymous and will help us improve.</t>
-  </si>
-  <si>
-    <t>Overall, how satisfied are you with your current job?</t>
-  </si>
-  <si>
-    <t>Very satisfied</t>
-  </si>
-  <si>
-    <t>Satisfied</t>
-  </si>
-  <si>
-    <t>Neutral</t>
-  </si>
-  <si>
-    <t>Dissatisfied</t>
-  </si>
-  <si>
-    <t>Are you working in week ends?</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>What areas do you think need improvement within the organization?</t>
-  </si>
-  <si>
-    <t>EventLink</t>
-  </si>
-  <si>
-    <t>EventVenue</t>
-  </si>
-  <si>
-    <t>Deep learning enhances efficiency and accuracy in documenting repetitive testing activities. AI in software testing minimizes human error and enhances fault detection capabilities.</t>
-  </si>
-  <si>
-    <t>The Forttuna Global Excellence Awards is dedicated to recognizing and honoring outstanding achievements. We take pride in acknowledging the contributions of individuals and companies that have significantly impacted their respective fields.
-Our Social Media Platforms 
-Instagram - https://www.instagram.com/forttunaawards
-YouTube - https://www.youtube.com/@ForttunaAwards
-Twitter - https://twitter.com/ForttunaAwards
-Facebook - https://www.facebook.com/forttunaaward?mibextid=LQQJ4d</t>
-  </si>
-  <si>
-    <t>ClubFees</t>
-  </si>
-  <si>
-    <t>new China Electronic Article Surveillance Market Size by Application</t>
-  </si>
-  <si>
-    <t>new The China Electronic Article Surveillance Market size is predicted to attain a valuation of USD 41.42 Billion in 2023, showing a compound annual growth rate (CAGR) of 9.04 percent from 2024 to 2031. Estimates place this value at USD 69.59 Billion by 2031.China Electronic Article Surveillance Market By Type:
-In the China Electronic Article Surveillance market, growth is evident through increased investments and evolving consumer preferences. Companies are leveraging advanced technologies and strategic initiatives to capture market share and drive expansion. With a focus on innovation and adaptability, businesses are responding to shifting trends and enhancing their offerings. This dynamic environment fosters robust growth, highlighting the market’s potential and its role in shaping future economic landscapes.</t>
-  </si>
-  <si>
-    <t>Job Description
-We are looking for an innovative technical lead to join our company. As the technical lead, you will oversee the companys technical team and all projects they undertake, identify risks, and develop work schedules. You should be able to work with your team and inspire them to reach their goals. Your core focus will be to stabilize and then migrate from our old system to a new version using the latest technologies.
-Roles and Responsibilities:
-Outline and implement a strategy to migrate away from Classic ASP application to a modern framework
-Conduct code reviews and define code quality standards
-Identify root cause issues and direct team on how to maintain and support existing ASP Classic applications.
-Define timelines and hold the team accountable for meeting deadlines
-Ensure the stability and performance of legacy systems. Develop initiative to increase automated test coverage
-Develop and implement new features using Typescript and modern frameworks.
-Work on both front-end and back-end components of the new system.
-Develop and maintain APIs and integration layers.
-Work with healthcare standards (e.g., HL7, FHIR) for interoperability.
-Oversee the development and integration projects.
-Coordinate between different teams (legacy, modern, security).
-Manage stakeholder expectations and communications.
-Translate business needs into technical specifications.
-Ensure projects are delivered on time and within budget.
-Qualifications:
-Knowledge of best practices in software development and agile methodologies. Desire to manage and teach.
-Strong experience with ASP Classic and related technologies.
-Familiarity with Windows infrastructure and IIS.
-Deep understanding of application monitoring. Experience with DataDog preferred.
-Ability to work with legacy databases and connectivity protocols.
-Proficiency in Typescript, Node.js, and modern JavaScript frameworks (React).
-Experience with back-end technologies such as Express.js and Microsoft SQL.
-Strong understanding of API development and integration.
-An understanding of healthcare interoperability standards will be an added advantage.
-Familiarity with both legacy system protocols and modern RESTful APIs.
-Strong analytical and problem-solving skills.
-Experience with automated testing.
-Familiarity with testing tools (e.g., Selenium, JUnit).
-Strong understanding of software development lifecycle.
-Excellent attention to detail and problem-solving skills.
-Experience with requirements gathering and documentation.
-Proven experience in project management
-Role: Technical Lead
-Industry Type: BPO / Call Centre
-Department: Engineering - Software &amp; QA
-Employment Type: Full Time, Permanent
-Role Category: Software Development
-Education
-UG: B.Tech/B.E. in Any Specialization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Production Testing club 2024 </t>
-  </si>
-  <si>
-    <t>2024 Production Testing  Awards event</t>
-  </si>
-  <si>
-    <t>The India hse summit &amp; Awards 2024 is a knowledge-based physical conference and the 7th edition of the flagship program hse summit by Synnex group. The 2-day summit strives to bring all key stakeholders—government officials, hse experts, industry associations and hse evangelists, technical leaders—together to discuss occupational safety and health &amp; EHS as a priority for companies while reiterating the significance and business benefits of investing in the health and safety of the workforce. This year the India hse summit &amp; awards 2024 is taking the initiative to spread awareness regarding the importance of occupational safety and health for the workforce in the ongoing covid19 pandemic with digitalization and technological solutions available to serve and save better</t>
-  </si>
-  <si>
-    <t>Vashi, Navi Mumbai</t>
-  </si>
-  <si>
     <t>FirstName</t>
   </si>
   <si>
     <t>LastName</t>
   </si>
   <si>
-    <t>CompanyEmailid</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Morrison</t>
-  </si>
-  <si>
-    <t>testuser0000000006@gmail.com</t>
+    <t>AdditionalFirstName</t>
+  </si>
+  <si>
+    <t>AdditionalLastName</t>
+  </si>
+  <si>
+    <t>AdditionalRelation</t>
+  </si>
+  <si>
+    <t>AdditionalPhone</t>
+  </si>
+  <si>
+    <t>AdditionalCurrentadd</t>
+  </si>
+  <si>
+    <t>AdditionalPermanentadd</t>
+  </si>
+  <si>
+    <t>Brother</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>Mary</t>
+  </si>
+  <si>
+    <t>testuser0000000012@gmail.com</t>
+  </si>
+  <si>
+    <t>Manya</t>
+  </si>
+  <si>
+    <t>Surve</t>
+  </si>
+  <si>
+    <t>Dongri</t>
+  </si>
+  <si>
+    <t>Dubai</t>
   </si>
 </sst>
 </file>
@@ -707,7 +522,7 @@
   <dimension ref="A1:AJ5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -715,11 +530,11 @@
     <col min="1" max="1" width="12.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.08984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.6328125" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="10" max="13" width="10.26953125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.54296875" bestFit="1" customWidth="1"/>
@@ -736,206 +551,116 @@
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>57</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>58</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
       <c r="AH1" s="2"/>
       <c r="AI1" s="2"/>
       <c r="AJ1" s="2"/>
     </row>
     <row r="2" spans="1:36" ht="87" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="D2" s="7">
-        <v>9100000006</v>
+        <v>91000000012</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>51</v>
+        <v>11</v>
+      </c>
+      <c r="H2" s="4">
+        <v>9898675403</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>56</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="4"/>
+      <c r="AC2" s="2"/>
       <c r="AD2" s="2"/>
-      <c r="AE2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="AG2" s="2">
-        <v>499</v>
-      </c>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="4"/>
+      <c r="AG2" s="2"/>
       <c r="AH2" s="2"/>
       <c r="AI2" s="2"/>
       <c r="AJ2" s="2"/>
@@ -1052,7 +777,7 @@
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Company Page Edit Additional Details and suite run profile creation
</commit_message>
<xml_diff>
--- a/TestData/Datasheet.xlsx
+++ b/TestData/Datasheet.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{FAA32C94-F658-419A-85A4-A803DE6E95E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1E2BD0BB-FCCA-43DE-A424-1FEE5688881A}"/>
+    <workbookView windowWidth="19200" windowHeight="6800"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -23,79 +29,79 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
     <t>MobileNumber</t>
   </si>
   <si>
+    <t>AdditionalFirstName</t>
+  </si>
+  <si>
+    <t>AdditionalLastName</t>
+  </si>
+  <si>
+    <t>AdditionalRelation</t>
+  </si>
+  <si>
+    <t>AdditionalPhone</t>
+  </si>
+  <si>
+    <t>AdditionalCurrentadd</t>
+  </si>
+  <si>
+    <t>AdditionalPermanentadd</t>
+  </si>
+  <si>
+    <t>Uday</t>
+  </si>
+  <si>
+    <t>Shetty</t>
+  </si>
+  <si>
+    <t>testuser0000000014@gmail.com</t>
+  </si>
+  <si>
+    <t>Manya</t>
+  </si>
+  <si>
+    <t>Surve</t>
+  </si>
+  <si>
+    <t>Brother</t>
+  </si>
+  <si>
+    <t>Dongri</t>
+  </si>
+  <si>
+    <t>Dubai</t>
+  </si>
+  <si>
     <t>mayurmore2706@gmail.com</t>
-  </si>
-  <si>
-    <t>FirstName</t>
-  </si>
-  <si>
-    <t>LastName</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>AdditionalFirstName</t>
-  </si>
-  <si>
-    <t>AdditionalLastName</t>
-  </si>
-  <si>
-    <t>AdditionalRelation</t>
-  </si>
-  <si>
-    <t>AdditionalPhone</t>
-  </si>
-  <si>
-    <t>AdditionalCurrentadd</t>
-  </si>
-  <si>
-    <t>AdditionalPermanentadd</t>
-  </si>
-  <si>
-    <t>Brother</t>
-  </si>
-  <si>
-    <t>Johnson</t>
-  </si>
-  <si>
-    <t>Mary</t>
-  </si>
-  <si>
-    <t>testuser0000000012@gmail.com</t>
-  </si>
-  <si>
-    <t>Manya</t>
-  </si>
-  <si>
-    <t>Surve</t>
-  </si>
-  <si>
-    <t>Dongri</t>
-  </si>
-  <si>
-    <t>Dubai</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -103,7 +109,7 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -111,10 +117,153 @@
       <sz val="10"/>
       <color rgb="FF2A00FF"/>
       <name val="Courier New"/>
-      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -127,8 +276,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -138,42 +473,282 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -183,20 +758,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -245,7 +862,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Display"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -278,26 +895,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Narrow"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -330,23 +930,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -508,77 +1091,72 @@
       </a:style>
     </a:lnDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91130ACC-1138-46D1-A908-9CE5228C9D06}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:AJ5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="4"/>
   <cols>
-    <col min="1" max="1" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.6328125" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="15" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="15" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6363636363636" customWidth="1"/>
+    <col min="2" max="2" width="24.3636363636364" customWidth="1"/>
+    <col min="3" max="3" width="15.1818181818182" customWidth="1"/>
+    <col min="4" max="4" width="13.0909090909091" customWidth="1"/>
+    <col min="5" max="5" width="31.6363636363636" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="9.54545454545454" customWidth="1"/>
+    <col min="8" max="8" width="10.8181818181818" customWidth="1"/>
+    <col min="9" max="9" width="11.1818181818182" customWidth="1"/>
+    <col min="10" max="13" width="10.2727272727273" customWidth="1"/>
+    <col min="14" max="14" width="9.54545454545454" customWidth="1"/>
+    <col min="15" max="15" width="10.2727272727273" customWidth="1"/>
+    <col min="16" max="16" width="12" customWidth="1"/>
+    <col min="17" max="20" width="15" customWidth="1"/>
+    <col min="21" max="21" width="12" customWidth="1"/>
+    <col min="22" max="23" width="15" customWidth="1"/>
+    <col min="24" max="24" width="12" customWidth="1"/>
+    <col min="25" max="25" width="10.5454545454545" customWidth="1"/>
+    <col min="26" max="26" width="10.6363636363636" customWidth="1"/>
+    <col min="32" max="32" width="10.2727272727273" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:36">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -607,36 +1185,36 @@
       <c r="AI1" s="2"/>
       <c r="AJ1" s="2"/>
     </row>
-    <row r="2" spans="1:36" ht="87" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" ht="87" customHeight="1" spans="1:36">
       <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="4">
+        <v>91000000014</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="7">
-        <v>91000000012</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="G2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="5">
+        <v>9898675403</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="4">
-        <v>9898675403</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
@@ -653,140 +1231,140 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
-      <c r="Z2" s="4"/>
+      <c r="Z2" s="5"/>
       <c r="AA2" s="2"/>
-      <c r="AB2" s="4"/>
+      <c r="AB2" s="5"/>
       <c r="AC2" s="2"/>
       <c r="AD2" s="2"/>
       <c r="AE2" s="2"/>
-      <c r="AF2" s="4"/>
+      <c r="AF2" s="5"/>
       <c r="AG2" s="2"/>
       <c r="AH2" s="2"/>
       <c r="AI2" s="2"/>
       <c r="AJ2" s="2"/>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A3" s="5">
+    <row r="3" spans="1:36">
+      <c r="A3" s="6">
         <v>0</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="6">
         <v>1</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="6">
         <v>2</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="6">
         <v>3</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="6">
         <v>4</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="6">
         <v>5</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="6">
         <v>6</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="6">
         <v>7</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="6">
         <v>8</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="6">
         <v>9</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3" s="6">
         <v>10</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3" s="6">
         <v>11</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3" s="6">
         <v>12</v>
       </c>
-      <c r="N3" s="5">
+      <c r="N3" s="6">
         <v>13</v>
       </c>
-      <c r="O3" s="5">
+      <c r="O3" s="6">
         <v>14</v>
       </c>
-      <c r="P3" s="5">
+      <c r="P3" s="6">
         <v>15</v>
       </c>
-      <c r="Q3" s="5">
+      <c r="Q3" s="6">
         <v>16</v>
       </c>
-      <c r="R3" s="5">
+      <c r="R3" s="6">
         <v>17</v>
       </c>
-      <c r="S3" s="5">
+      <c r="S3" s="6">
         <v>18</v>
       </c>
-      <c r="T3" s="5">
+      <c r="T3" s="6">
         <v>19</v>
       </c>
-      <c r="U3" s="5">
+      <c r="U3" s="6">
         <v>20</v>
       </c>
-      <c r="V3" s="5">
+      <c r="V3" s="6">
         <v>21</v>
       </c>
-      <c r="W3" s="5">
+      <c r="W3" s="6">
         <v>22</v>
       </c>
-      <c r="X3" s="5">
+      <c r="X3" s="6">
         <v>23</v>
       </c>
-      <c r="Y3" s="5">
+      <c r="Y3" s="6">
         <v>24</v>
       </c>
-      <c r="Z3" s="5">
+      <c r="Z3" s="6">
         <v>25</v>
       </c>
-      <c r="AA3" s="5">
+      <c r="AA3" s="6">
         <v>26</v>
       </c>
-      <c r="AB3" s="5">
+      <c r="AB3" s="6">
         <v>27</v>
       </c>
-      <c r="AC3" s="5">
+      <c r="AC3" s="6">
         <v>28</v>
       </c>
-      <c r="AD3" s="5">
+      <c r="AD3" s="6">
         <v>29</v>
       </c>
-      <c r="AE3" s="6">
+      <c r="AE3" s="7">
         <v>30</v>
       </c>
-      <c r="AF3" s="6">
+      <c r="AF3" s="7">
         <v>31</v>
       </c>
-      <c r="AG3" s="6">
+      <c r="AG3" s="7">
         <v>32</v>
       </c>
-      <c r="AH3" s="6">
+      <c r="AH3" s="7">
         <v>33</v>
       </c>
-      <c r="AI3" s="6">
+      <c r="AI3" s="7">
         <v>34</v>
       </c>
-      <c r="AJ3" s="6">
+      <c r="AJ3" s="7">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1">
       <c r="A5" s="3" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A5" r:id="rId1" xr:uid="{AA32F990-74EC-4ED5-8F90-EF79CE50017F}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{FC639CE8-F53C-45C8-8E8B-A19D7D162EFB}"/>
+    <hyperlink ref="A5" r:id="rId1" display="mayurmore2706@gmail.com"/>
+    <hyperlink ref="C2" r:id="rId2" display="testuser0000000014@gmail.com" tooltip="mailto:testuser0000000014@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>